<commit_message>
updated test administrtion feature
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/LoginDetails.xlsx
+++ b/src/test/resources/ExcelFiles/LoginDetails.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://focalpointk12-my.sharepoint.com/personal/gopi_pagadala_focalpointk12_com/Documents/FPK12 Automation-2024/FPK12-AssessmentCenter/src/test/resources/ExcelFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://focalpointk12-my.sharepoint.com/personal/suresh_rajaboina_focalpointk12_com/Documents/Focalpoint Automation/Benchmarks_AC/src/test/resources/ExcelFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="162" documentId="13_ncr:1_{6200E935-D564-4C0E-BA26-194115C14345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9764B68A-0102-40CB-84AE-FA94051FBD42}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{EEA9FC90-147D-4620-ADE8-69D720EFC016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8B73FD3-1F8B-4314-9553-78AF3BC24E47}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STAGE" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
   <si>
     <t>FirstName</t>
   </si>
@@ -71,15 +71,6 @@
     <t>fpk12student</t>
   </si>
   <si>
-    <t>2610</t>
-  </si>
-  <si>
-    <t>1283</t>
-  </si>
-  <si>
-    <t>4807</t>
-  </si>
-  <si>
     <t>fpadmin</t>
   </si>
   <si>
@@ -104,33 +95,6 @@
     <t>2613</t>
   </si>
   <si>
-    <t>FPK12School2965</t>
-  </si>
-  <si>
-    <t>FPK12Classroom2887</t>
-  </si>
-  <si>
-    <t>FPK12Section4407</t>
-  </si>
-  <si>
-    <t>1242</t>
-  </si>
-  <si>
-    <t>46</t>
-  </si>
-  <si>
-    <t>1299</t>
-  </si>
-  <si>
-    <t>FPK12School2102</t>
-  </si>
-  <si>
-    <t>FPK12Classroom923</t>
-  </si>
-  <si>
-    <t>FPK12Section1793</t>
-  </si>
-  <si>
     <t>493</t>
   </si>
   <si>
@@ -140,13 +104,40 @@
     <t>6629</t>
   </si>
   <si>
-    <t>FPK12School2044</t>
-  </si>
-  <si>
-    <t>FPK12Classroom4987</t>
-  </si>
-  <si>
-    <t>FPK12Section8844</t>
+    <t>Grade</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Grade 4</t>
+  </si>
+  <si>
+    <t>Biology</t>
+  </si>
+  <si>
+    <t>Testname</t>
+  </si>
+  <si>
+    <t>Automation Test</t>
+  </si>
+  <si>
+    <t>FPK12School5164</t>
+  </si>
+  <si>
+    <t>FPK12Classroom303</t>
+  </si>
+  <si>
+    <t>FPK12Section9660</t>
+  </si>
+  <si>
+    <t>FPK12School9336</t>
+  </si>
+  <si>
+    <t>FPK12Classroom9378</t>
+  </si>
+  <si>
+    <t>FPK12Section9591</t>
   </si>
 </sst>
 </file>
@@ -222,7 +213,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -257,6 +248,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <bottom style="thin"/>
     </border>
     <border>
@@ -320,13 +322,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyAlignment="true" applyBorder="true">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
     </xf>
   </cellXfs>
@@ -637,23 +639,23 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="30.0"/>
     <col min="2" max="2" customWidth="true" width="20.0"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="16.0"/>
-    <col min="4" max="4" customWidth="true" style="1" width="19.88671875"/>
-    <col min="5" max="5" customWidth="true" style="1" width="23.77734375"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="20.5546875"/>
-    <col min="8" max="8" customWidth="true" width="31.5546875"/>
+    <col min="4" max="4" customWidth="true" style="1" width="19.90625"/>
+    <col min="5" max="5" customWidth="true" style="1" width="23.81640625"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="20.54296875"/>
+    <col min="8" max="8" customWidth="true" width="31.54296875"/>
     <col min="11" max="11" customWidth="true" width="15.0"/>
-    <col min="12" max="12" customWidth="true" width="18.33203125"/>
+    <col min="12" max="12" customWidth="true" width="18.36328125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>3</v>
       </c>
@@ -681,19 +683,25 @@
       <c r="I1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="8"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-    </row>
-    <row r="2" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J1" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s" s="21">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s" s="21">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s" s="21">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>9</v>
@@ -713,11 +721,17 @@
       <c r="I2" s="14">
         <v>2024</v>
       </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J2" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -725,7 +739,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="F3" s="14">
         <v>1323</v>
@@ -739,7 +753,7 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -747,7 +761,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="F4" s="14">
         <v>1323</v>
@@ -761,7 +775,7 @@
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
@@ -769,7 +783,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="F5" s="14">
         <v>1323</v>
@@ -783,7 +797,7 @@
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
@@ -811,20 +825,20 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="30.0"/>
     <col min="2" max="2" customWidth="true" width="20.0"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="16.0"/>
-    <col min="4" max="4" customWidth="true" style="11" width="19.88671875"/>
-    <col min="5" max="5" customWidth="true" style="1" width="23.77734375"/>
-    <col min="7" max="7" customWidth="true" width="11.5546875"/>
-    <col min="8" max="8" customWidth="true" style="1" width="38.44140625"/>
+    <col min="4" max="4" customWidth="true" style="11" width="19.90625"/>
+    <col min="5" max="5" customWidth="true" style="1" width="23.81640625"/>
+    <col min="7" max="7" customWidth="true" width="11.54296875"/>
+    <col min="8" max="8" customWidth="true" style="1" width="38.453125"/>
     <col min="12" max="12" customWidth="true" width="15.0"/>
-    <col min="13" max="13" customWidth="true" width="18.33203125"/>
+    <col min="13" max="13" customWidth="true" width="18.36328125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>3</v>
       </c>
@@ -857,21 +871,21 @@
       <c r="L1" s="9"/>
       <c r="M1" s="9"/>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F2" s="2">
         <v>242</v>
@@ -890,7 +904,7 @@
       <c r="L2" s="2"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:13" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -898,7 +912,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F3" s="2">
         <v>242</v>
@@ -913,7 +927,7 @@
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -921,7 +935,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F4" s="2">
         <v>242</v>
@@ -936,7 +950,7 @@
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -944,7 +958,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F5" s="2">
         <v>242</v>
@@ -959,7 +973,7 @@
       <c r="L5" s="6"/>
       <c r="M5" s="6"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="18"/>
       <c r="B6" s="18"/>
       <c r="C6" s="18"/>

</xml_diff>

<commit_message>
Updated Assessment center Changes
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/LoginDetails.xlsx
+++ b/src/test/resources/ExcelFiles/LoginDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://focalpointk12-my.sharepoint.com/personal/gopi_pagadala_focalpointk12_com/Documents/FPK12 Automation-2024/FPK12-AssessmentCenter/src/test/resources/ExcelFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="162" documentId="13_ncr:1_{6200E935-D564-4C0E-BA26-194115C14345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9764B68A-0102-40CB-84AE-FA94051FBD42}"/>
+  <xr:revisionPtr revIDLastSave="175" documentId="13_ncr:1_{6200E935-D564-4C0E-BA26-194115C14345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B3CF720-9C74-49E9-A73C-754D09A3B359}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="92">
   <si>
     <t>FirstName</t>
   </si>
@@ -71,15 +71,6 @@
     <t>fpk12student</t>
   </si>
   <si>
-    <t>2610</t>
-  </si>
-  <si>
-    <t>1283</t>
-  </si>
-  <si>
-    <t>4807</t>
-  </si>
-  <si>
     <t>fpadmin</t>
   </si>
   <si>
@@ -104,49 +95,208 @@
     <t>2613</t>
   </si>
   <si>
-    <t>FPK12School2965</t>
-  </si>
-  <si>
-    <t>FPK12Classroom2887</t>
-  </si>
-  <si>
-    <t>FPK12Section4407</t>
-  </si>
-  <si>
-    <t>1242</t>
-  </si>
-  <si>
-    <t>46</t>
-  </si>
-  <si>
-    <t>1299</t>
-  </si>
-  <si>
-    <t>FPK12School2102</t>
-  </si>
-  <si>
-    <t>FPK12Classroom923</t>
-  </si>
-  <si>
-    <t>FPK12Section1793</t>
-  </si>
-  <si>
-    <t>493</t>
-  </si>
-  <si>
-    <t>9419</t>
-  </si>
-  <si>
-    <t>6629</t>
-  </si>
-  <si>
-    <t>FPK12School2044</t>
-  </si>
-  <si>
-    <t>FPK12Classroom4987</t>
-  </si>
-  <si>
-    <t>FPK12Section8844</t>
+    <t>0</t>
+  </si>
+  <si>
+    <t>3628</t>
+  </si>
+  <si>
+    <t>8007</t>
+  </si>
+  <si>
+    <t>FPK12School8433</t>
+  </si>
+  <si>
+    <t>FPK12Classroom7497</t>
+  </si>
+  <si>
+    <t>FPK12Section8962</t>
+  </si>
+  <si>
+    <t>TestName</t>
+  </si>
+  <si>
+    <t>Automation Test</t>
+  </si>
+  <si>
+    <t>FPK12School1355</t>
+  </si>
+  <si>
+    <t>FPK12Classroom9810</t>
+  </si>
+  <si>
+    <t>FPK12Section4735</t>
+  </si>
+  <si>
+    <t>FPK12School6260</t>
+  </si>
+  <si>
+    <t>FPK12Classroom8773</t>
+  </si>
+  <si>
+    <t>FPK12Section6809</t>
+  </si>
+  <si>
+    <t>FPK12School5336</t>
+  </si>
+  <si>
+    <t>FPK12Classroom5317</t>
+  </si>
+  <si>
+    <t>FPK12Section8155</t>
+  </si>
+  <si>
+    <t>FPK12School661</t>
+  </si>
+  <si>
+    <t>FPK12Classroom469</t>
+  </si>
+  <si>
+    <t>FPK12Section4805</t>
+  </si>
+  <si>
+    <t>529</t>
+  </si>
+  <si>
+    <t>3010</t>
+  </si>
+  <si>
+    <t>8041</t>
+  </si>
+  <si>
+    <t>FPK12School7501</t>
+  </si>
+  <si>
+    <t>FPK12Classroom7073</t>
+  </si>
+  <si>
+    <t>FPK12Section7276</t>
+  </si>
+  <si>
+    <t>4074</t>
+  </si>
+  <si>
+    <t>7398</t>
+  </si>
+  <si>
+    <t>5625</t>
+  </si>
+  <si>
+    <t>FPK12School3572</t>
+  </si>
+  <si>
+    <t>FPK12Classroom4985</t>
+  </si>
+  <si>
+    <t>FPK12Section4002</t>
+  </si>
+  <si>
+    <t>1684</t>
+  </si>
+  <si>
+    <t>7526</t>
+  </si>
+  <si>
+    <t>5430</t>
+  </si>
+  <si>
+    <t>FPK12School9251</t>
+  </si>
+  <si>
+    <t>FPK12Classroom1474</t>
+  </si>
+  <si>
+    <t>FPK12Section3047</t>
+  </si>
+  <si>
+    <t>9062</t>
+  </si>
+  <si>
+    <t>263</t>
+  </si>
+  <si>
+    <t>3748</t>
+  </si>
+  <si>
+    <t>FPK12School1968</t>
+  </si>
+  <si>
+    <t>FPK12Classroom9556</t>
+  </si>
+  <si>
+    <t>FPK12Section7200</t>
+  </si>
+  <si>
+    <t>6933</t>
+  </si>
+  <si>
+    <t>3164</t>
+  </si>
+  <si>
+    <t>5810</t>
+  </si>
+  <si>
+    <t>FPK12School5345</t>
+  </si>
+  <si>
+    <t>FPK12Classroom8434</t>
+  </si>
+  <si>
+    <t>FPK12Section9076</t>
+  </si>
+  <si>
+    <t>5773</t>
+  </si>
+  <si>
+    <t>6690</t>
+  </si>
+  <si>
+    <t>4636</t>
+  </si>
+  <si>
+    <t>FPK12School460</t>
+  </si>
+  <si>
+    <t>FPK12Classroom4783</t>
+  </si>
+  <si>
+    <t>FPK12Section4086</t>
+  </si>
+  <si>
+    <t>5343</t>
+  </si>
+  <si>
+    <t>2896</t>
+  </si>
+  <si>
+    <t>316</t>
+  </si>
+  <si>
+    <t>FPK12School2308</t>
+  </si>
+  <si>
+    <t>FPK12Classroom1682</t>
+  </si>
+  <si>
+    <t>FPK12Section524</t>
+  </si>
+  <si>
+    <t>FPK12School9124</t>
+  </si>
+  <si>
+    <t>FPK12Classroom8864</t>
+  </si>
+  <si>
+    <t>FPK12Section2133</t>
+  </si>
+  <si>
+    <t>789</t>
+  </si>
+  <si>
+    <t>5338</t>
+  </si>
+  <si>
+    <t>3587</t>
   </si>
 </sst>
 </file>
@@ -222,7 +372,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -257,6 +407,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <bottom style="thin"/>
     </border>
     <border>
@@ -268,7 +429,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -320,13 +481,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyAlignment="true" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyAlignment="true" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyAlignment="true" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
     </xf>
   </cellXfs>
@@ -345,6 +539,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -637,7 +835,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -649,6 +847,7 @@
     <col min="5" max="5" customWidth="true" style="1" width="23.77734375"/>
     <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="20.5546875"/>
     <col min="8" max="8" customWidth="true" width="31.5546875"/>
+    <col min="10" max="10" customWidth="true" width="16.33203125"/>
     <col min="11" max="11" customWidth="true" width="15.0"/>
     <col min="12" max="12" customWidth="true" width="18.33203125"/>
   </cols>
@@ -681,19 +880,21 @@
       <c r="I1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="8"/>
+      <c r="J1" s="20" t="s">
+        <v>30</v>
+      </c>
       <c r="K1" s="9"/>
       <c r="L1" s="9"/>
     </row>
     <row r="2" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="21">
-        <v>39</v>
-      </c>
-      <c r="B2" t="s" s="21">
-        <v>40</v>
-      </c>
-      <c r="C2" t="s" s="21">
-        <v>41</v>
+      <c r="A2" t="s" s="32">
+        <v>86</v>
+      </c>
+      <c r="B2" t="s" s="32">
+        <v>87</v>
+      </c>
+      <c r="C2" t="s" s="32">
+        <v>88</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>9</v>
@@ -713,7 +914,9 @@
       <c r="I2" s="14">
         <v>2024</v>
       </c>
-      <c r="J2" s="6"/>
+      <c r="J2" s="14" t="s">
+        <v>31</v>
+      </c>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
     </row>
@@ -725,7 +928,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>36</v>
+        <v>89</v>
       </c>
       <c r="F3" s="14">
         <v>1323</v>
@@ -747,7 +950,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>37</v>
+        <v>90</v>
       </c>
       <c r="F4" s="14">
         <v>1323</v>
@@ -769,7 +972,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>38</v>
+        <v>91</v>
       </c>
       <c r="F5" s="14">
         <v>1323</v>
@@ -859,19 +1062,19 @@
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F2" s="2">
         <v>242</v>
@@ -898,7 +1101,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F3" s="2">
         <v>242</v>
@@ -921,7 +1124,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F4" s="2">
         <v>242</v>
@@ -944,7 +1147,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F5" s="2">
         <v>242</v>

</xml_diff>

<commit_message>
Enhancing Quiz Creation Script
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/LoginDetails.xlsx
+++ b/src/test/resources/ExcelFiles/LoginDetails.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://focalpointk12-my.sharepoint.com/personal/gopi_pagadala_focalpointk12_com/Documents/FPK12 Automation-2024/FPK12-AssessmentCenter/src/test/resources/ExcelFiles/"/>
     </mc:Choice>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
   <si>
     <t>FirstName</t>
   </si>
@@ -95,190 +95,10 @@
     <t>2613</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>3628</t>
-  </si>
-  <si>
-    <t>8007</t>
-  </si>
-  <si>
-    <t>FPK12School8433</t>
-  </si>
-  <si>
-    <t>FPK12Classroom7497</t>
-  </si>
-  <si>
-    <t>FPK12Section8962</t>
-  </si>
-  <si>
     <t>TestName</t>
   </si>
   <si>
     <t>Automation Test</t>
-  </si>
-  <si>
-    <t>FPK12School1355</t>
-  </si>
-  <si>
-    <t>FPK12Classroom9810</t>
-  </si>
-  <si>
-    <t>FPK12Section4735</t>
-  </si>
-  <si>
-    <t>FPK12School6260</t>
-  </si>
-  <si>
-    <t>FPK12Classroom8773</t>
-  </si>
-  <si>
-    <t>FPK12Section6809</t>
-  </si>
-  <si>
-    <t>FPK12School5336</t>
-  </si>
-  <si>
-    <t>FPK12Classroom5317</t>
-  </si>
-  <si>
-    <t>FPK12Section8155</t>
-  </si>
-  <si>
-    <t>FPK12School661</t>
-  </si>
-  <si>
-    <t>FPK12Classroom469</t>
-  </si>
-  <si>
-    <t>FPK12Section4805</t>
-  </si>
-  <si>
-    <t>529</t>
-  </si>
-  <si>
-    <t>3010</t>
-  </si>
-  <si>
-    <t>8041</t>
-  </si>
-  <si>
-    <t>FPK12School7501</t>
-  </si>
-  <si>
-    <t>FPK12Classroom7073</t>
-  </si>
-  <si>
-    <t>FPK12Section7276</t>
-  </si>
-  <si>
-    <t>4074</t>
-  </si>
-  <si>
-    <t>7398</t>
-  </si>
-  <si>
-    <t>5625</t>
-  </si>
-  <si>
-    <t>FPK12School3572</t>
-  </si>
-  <si>
-    <t>FPK12Classroom4985</t>
-  </si>
-  <si>
-    <t>FPK12Section4002</t>
-  </si>
-  <si>
-    <t>1684</t>
-  </si>
-  <si>
-    <t>7526</t>
-  </si>
-  <si>
-    <t>5430</t>
-  </si>
-  <si>
-    <t>FPK12School9251</t>
-  </si>
-  <si>
-    <t>FPK12Classroom1474</t>
-  </si>
-  <si>
-    <t>FPK12Section3047</t>
-  </si>
-  <si>
-    <t>9062</t>
-  </si>
-  <si>
-    <t>263</t>
-  </si>
-  <si>
-    <t>3748</t>
-  </si>
-  <si>
-    <t>FPK12School1968</t>
-  </si>
-  <si>
-    <t>FPK12Classroom9556</t>
-  </si>
-  <si>
-    <t>FPK12Section7200</t>
-  </si>
-  <si>
-    <t>6933</t>
-  </si>
-  <si>
-    <t>3164</t>
-  </si>
-  <si>
-    <t>5810</t>
-  </si>
-  <si>
-    <t>FPK12School5345</t>
-  </si>
-  <si>
-    <t>FPK12Classroom8434</t>
-  </si>
-  <si>
-    <t>FPK12Section9076</t>
-  </si>
-  <si>
-    <t>5773</t>
-  </si>
-  <si>
-    <t>6690</t>
-  </si>
-  <si>
-    <t>4636</t>
-  </si>
-  <si>
-    <t>FPK12School460</t>
-  </si>
-  <si>
-    <t>FPK12Classroom4783</t>
-  </si>
-  <si>
-    <t>FPK12Section4086</t>
-  </si>
-  <si>
-    <t>5343</t>
-  </si>
-  <si>
-    <t>2896</t>
-  </si>
-  <si>
-    <t>316</t>
-  </si>
-  <si>
-    <t>FPK12School2308</t>
-  </si>
-  <si>
-    <t>FPK12Classroom1682</t>
-  </si>
-  <si>
-    <t>FPK12Section524</t>
   </si>
   <si>
     <t>FPK12School9124</t>
@@ -303,7 +123,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -372,7 +191,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -417,19 +236,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <right style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -481,47 +293,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
-      <alignment vertical="center" horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -835,21 +611,21 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="30.0"/>
-    <col min="2" max="2" customWidth="true" width="20.0"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.0"/>
-    <col min="4" max="4" customWidth="true" style="1" width="19.88671875"/>
-    <col min="5" max="5" customWidth="true" style="1" width="23.77734375"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="20.5546875"/>
-    <col min="8" max="8" customWidth="true" width="31.5546875"/>
-    <col min="10" max="10" customWidth="true" width="16.33203125"/>
-    <col min="11" max="11" customWidth="true" width="15.0"/>
-    <col min="12" max="12" customWidth="true" width="18.33203125"/>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.5546875" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" customWidth="1"/>
+    <col min="11" max="11" width="15" customWidth="1"/>
+    <col min="12" max="12" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -880,21 +656,21 @@
       <c r="I1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="20" t="s">
-        <v>30</v>
+      <c r="J1" s="19" t="s">
+        <v>24</v>
       </c>
       <c r="K1" s="9"/>
       <c r="L1" s="9"/>
     </row>
     <row r="2" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="32">
-        <v>86</v>
-      </c>
-      <c r="B2" t="s" s="32">
-        <v>87</v>
-      </c>
-      <c r="C2" t="s" s="32">
-        <v>88</v>
+      <c r="A2" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>28</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>9</v>
@@ -915,7 +691,7 @@
         <v>2024</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
@@ -928,7 +704,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>89</v>
+        <v>29</v>
       </c>
       <c r="F3" s="14">
         <v>1323</v>
@@ -950,7 +726,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="F4" s="14">
         <v>1323</v>
@@ -972,7 +748,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>91</v>
+        <v>31</v>
       </c>
       <c r="F5" s="14">
         <v>1323</v>
@@ -1016,15 +792,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="30.0"/>
-    <col min="2" max="2" customWidth="true" width="20.0"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.0"/>
-    <col min="4" max="4" customWidth="true" style="11" width="19.88671875"/>
-    <col min="5" max="5" customWidth="true" style="1" width="23.77734375"/>
-    <col min="7" max="7" customWidth="true" width="11.5546875"/>
-    <col min="8" max="8" customWidth="true" style="1" width="38.44140625"/>
-    <col min="12" max="12" customWidth="true" width="15.0"/>
-    <col min="13" max="13" customWidth="true" width="18.33203125"/>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.88671875" style="11" customWidth="1"/>
+    <col min="5" max="5" width="23.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" customWidth="1"/>
+    <col min="8" max="8" width="38.44140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="15" customWidth="1"/>
+    <col min="13" max="13" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Handling timeout Exception Code
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/LoginDetails.xlsx
+++ b/src/test/resources/ExcelFiles/LoginDetails.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="89">
   <si>
     <t>FirstName</t>
   </si>
@@ -267,6 +267,27 @@
   </si>
   <si>
     <t>50691</t>
+  </si>
+  <si>
+    <t>FPK12School48551</t>
+  </si>
+  <si>
+    <t>FPK12Classroom93735</t>
+  </si>
+  <si>
+    <t>FPK12Section42833</t>
+  </si>
+  <si>
+    <t>11381</t>
+  </si>
+  <si>
+    <t>3850</t>
+  </si>
+  <si>
+    <t>57166</t>
+  </si>
+  <si>
+    <t>7444</t>
   </si>
 </sst>
 </file>
@@ -399,7 +420,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -456,6 +477,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
@@ -846,14 +870,14 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="27">
-        <v>76</v>
-      </c>
-      <c r="B2" t="s" s="27">
-        <v>77</v>
-      </c>
-      <c r="C2" t="s" s="27">
-        <v>78</v>
+      <c r="A2" t="s" s="28">
+        <v>82</v>
+      </c>
+      <c r="B2" t="s" s="28">
+        <v>83</v>
+      </c>
+      <c r="C2" t="s" s="28">
+        <v>84</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>9</v>
@@ -891,7 +915,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="F3" s="13">
         <v>1323</v>
@@ -909,11 +933,9 @@
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
-      <c r="D4" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="F4" s="13">
         <v>1323</v>
@@ -931,11 +953,9 @@
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
-      <c r="D5" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
       <c r="F5" s="13">
         <v>1323</v>

</xml_diff>

<commit_message>
Stale Element Exception handling
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/LoginDetails.xlsx
+++ b/src/test/resources/ExcelFiles/LoginDetails.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="98">
   <si>
     <t>FirstName</t>
   </si>
@@ -288,6 +288,33 @@
   </si>
   <si>
     <t>7444</t>
+  </si>
+  <si>
+    <t>FPK12School60560</t>
+  </si>
+  <si>
+    <t>FPK12Classroom30852</t>
+  </si>
+  <si>
+    <t>FPK12Section76423</t>
+  </si>
+  <si>
+    <t>FPK12School98753</t>
+  </si>
+  <si>
+    <t>FPK12Classroom85288</t>
+  </si>
+  <si>
+    <t>FPK12Section84910</t>
+  </si>
+  <si>
+    <t>76982</t>
+  </si>
+  <si>
+    <t>91009</t>
+  </si>
+  <si>
+    <t>95746</t>
   </si>
 </sst>
 </file>
@@ -420,7 +447,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -477,6 +504,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
@@ -870,14 +903,14 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="28">
-        <v>82</v>
-      </c>
-      <c r="B2" t="s" s="28">
-        <v>83</v>
-      </c>
-      <c r="C2" t="s" s="28">
-        <v>84</v>
+      <c r="A2" t="s" s="30">
+        <v>92</v>
+      </c>
+      <c r="B2" t="s" s="30">
+        <v>93</v>
+      </c>
+      <c r="C2" t="s" s="30">
+        <v>94</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>9</v>
@@ -915,7 +948,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="F3" s="13">
         <v>1323</v>
@@ -933,9 +966,11 @@
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="E4" s="2" t="s">
-        <v>43</v>
+        <v>96</v>
       </c>
       <c r="F4" s="13">
         <v>1323</v>
@@ -953,9 +988,11 @@
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="E5" s="2" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
       <c r="F5" s="13">
         <v>1323</v>

</xml_diff>

<commit_message>
Implementing Student Report card Storing in Folder
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/LoginDetails.xlsx
+++ b/src/test/resources/ExcelFiles/LoginDetails.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="110">
   <si>
     <t>FirstName</t>
   </si>
@@ -315,6 +315,42 @@
   </si>
   <si>
     <t>95746</t>
+  </si>
+  <si>
+    <t>FPK12School71985</t>
+  </si>
+  <si>
+    <t>FPK12Classroom60511</t>
+  </si>
+  <si>
+    <t>FPK12Section76666</t>
+  </si>
+  <si>
+    <t>30721</t>
+  </si>
+  <si>
+    <t>8889</t>
+  </si>
+  <si>
+    <t>21432</t>
+  </si>
+  <si>
+    <t>FPK12School16006</t>
+  </si>
+  <si>
+    <t>FPK12Classroom23482</t>
+  </si>
+  <si>
+    <t>FPK12Section35176</t>
+  </si>
+  <si>
+    <t>40247</t>
+  </si>
+  <si>
+    <t>67235</t>
+  </si>
+  <si>
+    <t>60032</t>
   </si>
 </sst>
 </file>
@@ -447,7 +483,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -504,6 +540,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment vertical="center" horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
@@ -903,14 +945,14 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="30">
-        <v>92</v>
-      </c>
-      <c r="B2" t="s" s="30">
-        <v>93</v>
-      </c>
-      <c r="C2" t="s" s="30">
-        <v>94</v>
+      <c r="A2" t="s" s="32">
+        <v>104</v>
+      </c>
+      <c r="B2" t="s" s="32">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s" s="32">
+        <v>106</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>9</v>
@@ -948,7 +990,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="F3" s="13">
         <v>1323</v>
@@ -970,7 +1012,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="F4" s="13">
         <v>1323</v>
@@ -992,7 +1034,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="F5" s="13">
         <v>1323</v>

</xml_diff>